<commit_message>
doc: se modifica archivo de usuarios y permisos
</commit_message>
<xml_diff>
--- a/Bases de datos/Documentación/Creacion de users.xlsx
+++ b/Bases de datos/Documentación/Creacion de users.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucho\Documents\GitHub\Repositorio-de-equipo-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANTIAGO\Desktop\Repositorio-de-equipo-3\Bases de datos\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D45D75-4EC7-4A84-A4C5-67D73C28C08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="-120" windowWidth="28065" windowHeight="16440" xr2:uid="{915D0D72-919F-4EC8-B87C-0E661B558825}"/>
+    <workbookView xWindow="1785" yWindow="-120" windowWidth="28065" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>TABLAS</t>
   </si>
@@ -102,9 +101,6 @@
     <t xml:space="preserve">Read </t>
   </si>
   <si>
-    <t>Vigilante Minuta</t>
-  </si>
-  <si>
     <t>Registro minuta</t>
   </si>
   <si>
@@ -153,18 +149,9 @@
     <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.incidente TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.programas TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
-    <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'rositarpelea100'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>santiago.cruzuwu25</t>
   </si>
   <si>
@@ -204,9 +191,6 @@
     <t>GRANT SELECT, UPDATE ON sena.asistencia TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.jornada TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.recursos TO 'jtavarez92'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
@@ -241,12 +225,18 @@
   </si>
   <si>
     <t>GRANT SELECT, UPDATE ON sena.modalidad TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
+  </si>
+  <si>
+    <t>Guarda de Seguridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Read, Update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,7 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -461,25 +451,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -802,11 +798,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914852BE-CF9F-4359-89B7-1C4A7749B8FD}">
-  <dimension ref="A1:P30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +845,7 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -859,20 +855,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
@@ -883,13 +879,13 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>20</v>
@@ -897,305 +893,305 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
-      <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="7" t="s">
-        <v>41</v>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="14" t="s">
+    </row>
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="14" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="P13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14" t="s">
+      <c r="C15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="3" t="s">
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="14" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>9</v>
@@ -1204,13 +1200,13 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
       <c r="B24" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -1219,13 +1215,13 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
       <c r="B25" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>9</v>
@@ -1234,101 +1230,42 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="A18:A26"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{24FD22E6-9CDE-4D49-B194-D2C49C14D557}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc: se elimina fila no necesaria
</commit_message>
<xml_diff>
--- a/Bases de datos/Documentación/Creacion de users.xlsx
+++ b/Bases de datos/Documentación/Creacion de users.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SANTIAGO\Desktop\Repositorio-de-equipo-3\Bases de datos\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamil\OneDrive\Documentos\Repositorio-de-equipo-3\Bases de datos\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD3E4E-1D77-4872-82ED-C96E2B2BA7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="-120" windowWidth="28065" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>TABLAS</t>
   </si>
@@ -212,9 +204,6 @@
     <t>GRANT SELECT, UPDATE ON sena.incidente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
-    <t>GRANT SELECT, UPDATE ON sena.minutas TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
-  </si>
-  <si>
     <t>GRANT SELECT, UPDATE ON sena.ambiente TO 'javier.pineda21'@'localhost'; FLUSH PRIVILEGES;</t>
   </si>
   <si>
@@ -228,15 +217,12 @@
   </si>
   <si>
     <t>Guarda de Seguridad</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Read, Update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +381,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,12 +416,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -451,8 +431,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -469,15 +452,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -798,11 +785,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +832,7 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -857,7 +844,7 @@
       <c r="D2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -868,7 +855,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
@@ -883,7 +870,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
@@ -893,13 +880,13 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>64</v>
+      <c r="A5" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>22</v>
@@ -913,15 +900,15 @@
       <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
@@ -936,7 +923,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
@@ -946,12 +933,12 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -966,30 +953,30 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1007,22 +994,22 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1024,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
@@ -1047,66 +1034,66 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="27" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="25"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1121,7 +1108,7 @@
       <c r="E18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="14" t="s">
         <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1129,7 +1116,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="11" t="s">
         <v>15</v>
       </c>
@@ -1139,12 +1126,12 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1146,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="11" t="s">
         <v>16</v>
       </c>
@@ -1169,29 +1156,29 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="3" t="s">
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
       <c r="B23" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>9</v>
@@ -1199,71 +1186,59 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="3" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="11" t="s">
-        <v>18</v>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="3" t="s">
-        <v>63</v>
-      </c>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="A18:A26"/>
-    <mergeCell ref="C15:C17"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="C15:C17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>